<commit_message>
exclusion to all white milk brands
</commit_message>
<xml_diff>
--- a/Projects/CCAAU/Data/template.xlsx
+++ b/Projects/CCAAU/Data/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="23">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -62,7 +62,14 @@
     <t xml:space="preserve">2,4,2.25,2.4,10,3</t>
   </si>
   <si>
-    <t xml:space="preserve">WHITE MILK,Irrelevant,General</t>
+    <t xml:space="preserve">Irrelevant,General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2 White Milk,Dairy Farmers White Milk,Pauls White Milk,Other Dairy
+</t>
   </si>
   <si>
     <t xml:space="preserve">Share of Shelf by Linear</t>
@@ -71,13 +78,17 @@
     <t xml:space="preserve">FLAVOURED MILK, 07- JUICE</t>
   </si>
   <si>
+    <t xml:space="preserve">A2 White Milk,Dairy Farmers White Milk,Pauls White Milk,Other Dairy  </t>
+  </si>
+  <si>
     <t xml:space="preserve">Denominator</t>
   </si>
   <si>
     <t xml:space="preserve"> FLAVOURED MILK,07- JUICE</t>
   </si>
   <si>
-    <t xml:space="preserve">brand</t>
+    <t xml:space="preserve"> 
+</t>
   </si>
   <si>
     <t xml:space="preserve">Empty</t>
@@ -219,7 +230,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -246,6 +257,14 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -326,18 +345,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="27.8061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,30 +419,26 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -433,18 +447,22 @@
         <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>9</v>
@@ -458,31 +476,27 @@
     </row>
     <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>12</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -496,23 +510,100 @@
     </row>
     <row r="9" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -533,18 +624,17 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,10 +665,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -588,45 +678,45 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>

</xml_diff>

<commit_message>
PROS-7407 CCANZ Linear SOS measurement chagne
</commit_message>
<xml_diff>
--- a/Projects/CCAAU/Data/template.xlsx
+++ b/Projects/CCAAU/Data/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">category</t>
   </si>
   <si>
-    <t xml:space="preserve">FLAVOURED MILK,07- JUICE</t>
+    <t xml:space="preserve">07- JUICE,09- Dairy</t>
   </si>
   <si>
     <t xml:space="preserve">size</t>
@@ -74,13 +74,13 @@
     <t xml:space="preserve">Share of Shelf by Linear</t>
   </si>
   <si>
-    <t xml:space="preserve">FLAVOURED MILK, 07- JUICE</t>
+    <t xml:space="preserve">09- Dairy, 07- JUICE</t>
   </si>
   <si>
     <t xml:space="preserve">Denominator</t>
   </si>
   <si>
-    <t xml:space="preserve"> FLAVOURED MILK,07- JUICE</t>
+    <t xml:space="preserve">09- Dairy,07- JUICE</t>
   </si>
   <si>
     <t xml:space="preserve"> 
@@ -97,7 +97,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -118,6 +118,33 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="16"/>
@@ -127,13 +154,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -145,12 +165,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -228,49 +242,69 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -353,263 +387,267 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.1887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="47.8418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.26020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6" t="s">
+      <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="7"/>
+      <c r="F12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="9" t="s">
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -631,103 +669,103 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
PROS-7407 brand exlcude removed
</commit_message>
<xml_diff>
--- a/Projects/CCAAU/Data/template.xlsx
+++ b/Projects/CCAAU/Data/template.xlsx
@@ -68,7 +68,7 @@
     <t xml:space="preserve">brand_name</t>
   </si>
   <si>
-    <t xml:space="preserve">A2 White Milk,Dairy Farmers White Milk,Pauls White Milk,Other Dairy</t>
+    <t xml:space="preserve">,</t>
   </si>
   <si>
     <t xml:space="preserve">Share of Shelf by Linear</t>
@@ -388,19 +388,19 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.1887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.0459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="47.8418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.5969387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.26020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,12 +675,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Scene type Bay Count kpi
</commit_message>
<xml_diff>
--- a/Projects/CCAAU/Data/template.xlsx
+++ b/Projects/CCAAU/Data/template.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Include" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="BayCountKPI" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="30">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -88,6 +89,30 @@
   </si>
   <si>
     <t xml:space="preserve">Empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAY_COUNT_BY_SCENE_TYPE_IN_WHOLE_STORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCA-Express checkout cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCA-On Exit Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCA-Standard checkout cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster branded cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCA 2 Door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.1 Farmers Union Cooler</t>
   </si>
 </sst>
 </file>
@@ -97,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -163,6 +188,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -246,7 +278,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -305,6 +337,18 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -387,20 +431,20 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.8469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.7091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="47.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.04081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.95408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="11.1581632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,12 +719,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.52040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -776,4 +820,74 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding bay count kpi
</commit_message>
<xml_diff>
--- a/Projects/CCAAU/Data/template.xlsx
+++ b/Projects/CCAAU/Data/template.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Include" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="BayCountKPI" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -88,6 +89,18 @@
   </si>
   <si>
     <t xml:space="preserve">Empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scene Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAY_COUNT_BY_SCENE_TYPE_IN_WHOLE_STORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
   </si>
 </sst>
 </file>
@@ -97,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -166,8 +179,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,8 +200,14 @@
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -217,6 +243,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -246,7 +279,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -305,6 +338,14 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -387,20 +428,20 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.7091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.1683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,12 +716,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -776,4 +817,48 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Template for CCAAU Bay Count KPI changed
</commit_message>
<xml_diff>
--- a/Projects/CCAAU/Data/template.xlsx
+++ b/Projects/CCAAU/Data/template.xlsx
@@ -100,7 +100,7 @@
     <t xml:space="preserve">BAY_COUNT_BY_SCENE_TYPE_IN_WHOLE_STORE</t>
   </si>
   <si>
-    <t xml:space="preserve">*</t>
+    <t xml:space="preserve">CCA - STANDARD LONG LANE CHECKOUT,CCA - EXPRESS CHECKOUT,CCA - SELF CHECK OUT,CCA - OTHER - FRONT OF STORE,CCA - INDIES - REST OF STORE,Competitor - STANDARD LONG LANE CHECKOUT,Competitor - EXPRESS CHECKOUT,Competitor - SELF CHECK OUT,Competitor - OTHER - FRONT OF STORE,Competitor - INDIES - REST OF STORE</t>
   </si>
 </sst>
 </file>
@@ -436,11 +436,11 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.280612244898"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.59183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.3214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.04081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.84183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.3571428571429"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
@@ -716,12 +716,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4336734693878"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.719387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.39795918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,13 +827,14 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -844,7 +845,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="124" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
adding template without tests
</commit_message>
<xml_diff>
--- a/Projects/CCAAU/Data/template.xlsx
+++ b/Projects/CCAAU/Data/template.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Include" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="BayCountKPI" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -60,7 +60,7 @@
     <t xml:space="preserve">size</t>
   </si>
   <si>
-    <t xml:space="preserve">2,4,2.25,2.4,10,3</t>
+    <t xml:space="preserve">2,4,2.25,2.4,10,3,2000,2400</t>
   </si>
   <si>
     <t xml:space="preserve">Irrelevant,General</t>
@@ -428,23 +428,23 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.59183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.3214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.04081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.84183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="10.8010204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="46.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="10.82"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -467,7 +467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -488,7 +488,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -505,7 +505,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -522,7 +522,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -543,7 +543,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -560,7 +560,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -577,7 +577,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -594,7 +594,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -615,7 +615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -632,7 +632,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -649,7 +649,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -670,7 +670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -687,7 +687,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
@@ -695,7 +695,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -710,21 +710,21 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.719387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.39795918367347"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -744,7 +744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -760,7 +760,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -776,7 +776,7 @@
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
@@ -792,7 +792,7 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
         <v>16</v>
       </c>
@@ -811,7 +811,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -826,18 +826,18 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
         <v>22</v>
       </c>
@@ -856,7 +856,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>